<commit_message>
Criado validações na tela de [Conciliacao Bancaria]
</commit_message>
<xml_diff>
--- a/cypress/downloads/Pagamentos  por Conta Bancária.xlsx
+++ b/cypress/downloads/Pagamentos  por Conta Bancária.xlsx
@@ -247,14 +247,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="35.57" min="1" max="1" customWidth="1"/>
-    <col width="40.71" min="2" max="2" customWidth="1"/>
-    <col width="39.29" min="3" max="3" customWidth="1"/>
-    <col width="28.57" min="4" max="4" customWidth="1"/>
-    <col width="38.14" min="5" max="5" customWidth="1"/>
-    <col width="24.43" min="6" max="6" customWidth="1"/>
-    <col width="23.57" min="7" max="7" customWidth="1"/>
-    <col width="21.71" min="8" max="8" customWidth="1"/>
+    <col width="35.86" min="1" max="1" customWidth="1"/>
+    <col width="41.14" min="2" max="2" customWidth="1"/>
+    <col width="39.71" min="3" max="3" customWidth="1"/>
+    <col width="28.86" min="4" max="4" customWidth="1"/>
+    <col width="38.43" min="5" max="5" customWidth="1"/>
+    <col width="24.71" min="6" max="6" customWidth="1"/>
+    <col width="23.86" min="7" max="7" customWidth="1"/>
+    <col width="22" min="8" max="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" outlineLevel="0" x14ac:dyDescent="0.25">

</xml_diff>